<commit_message>
Fix testplan for missing connector tests
Fix the test plan to better test the Grove connectors. The A0 to A6
Arduino pins were not getting exercised. Also, the 96B pins were not
getting effectively tested. Update the test sketch to include the A0 to
A6 pins, and update the testplan to match.

Signed-off-by: Grant Likely <grant.likely@linaro.org>
</commit_message>
<xml_diff>
--- a/96boards-sensors-bom-test.xlsx
+++ b/96boards-sensors-bom-test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="237">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -649,7 +649,7 @@
     <t>g.</t>
   </si>
   <si>
-    <t>Program ATMEGA328 using ISP header with standard Arduino UNO bootloader</t>
+    <t>Program supplied Arduino “BlinkAll” sketch onto ATMEGA328 using ISP header</t>
   </si>
   <si>
     <t>h.</t>
@@ -667,67 +667,61 @@
     <t>j.</t>
   </si>
   <si>
-    <t>Using Arduino IDE, program UUT with example “Blink” sketch. You will need to manually press the “reset” button on the UUT to initiate programming</t>
+    <t>Using serial terminal emulator on PC, verify ATMEGA is responding to serial traffic</t>
   </si>
   <si>
     <t>k.</t>
   </si>
   <si>
-    <t>Verify UUT LED D3 (PB5) is flashing.</t>
+    <t>Connect GROVE LED modules to connectors P8-11, P14-16 and P18. 8 modules in all (or use a single module to test each connector one at a time.)</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>Seeed's regular GROVE LED modules only use a single GPIO signal on the GROVE connector. For complete testing we would want a Grove module with 2 LEDs so that both signals get tested.</t>
   </si>
   <si>
     <t>l.</t>
   </si>
   <si>
-    <t>Using Arduino IDE, program UUT with provided “BlinkAll” sketch. You will need to manually press the “reset” button on the UUT to initiate programming</t>
+    <t>Verify all LEDs on GROVE modules are flashing.</t>
   </si>
   <si>
     <t>m.</t>
   </si>
   <si>
-    <t>Connect GROVE LED modules to connectors P7-11 and P14-18. 10 modules in all (or use a single module to test each connector one at a time.)</t>
-  </si>
-  <si>
-    <t>Note:</t>
-  </si>
-  <si>
-    <t>Seeed's regular GROVE LED modules only use a single GPIO signal on the GROVE connector. For complete testing we would want a Grove module with 2 LEDs so that both signals get tested.</t>
+    <t>Connect GROVE cable from P14 to P12</t>
   </si>
   <si>
     <t>n.</t>
   </si>
   <si>
-    <t>Verify all LEDs on GROVE modules are flashing.</t>
+    <t>Connect GROVE cable from P15 to P19</t>
   </si>
   <si>
     <t>o.</t>
   </si>
   <si>
-    <t>Connect GROVE cable from P11 to P13</t>
+    <t>Verify UUT LEDs are flashing: D4-D7 (GPIOA-GPIOD)</t>
   </si>
   <si>
     <t>p.</t>
   </si>
   <si>
-    <t>Connect GROVE cable from P18 to P20</t>
+    <t>Connect GROVE LED modules to P13 and P20</t>
   </si>
   <si>
     <t>q.</t>
   </si>
   <si>
-    <t>Verify UUT LEDs are flashing: D4-D7 (GPIOA-GPIOD)</t>
+    <t>Verify all LEDs on GROVE modules are flashing</t>
   </si>
   <si>
     <t>r.</t>
   </si>
   <si>
-    <t>Connect GROVE LED modules to P14 and P29</t>
-  </si>
-  <si>
-    <t>s.</t>
-  </si>
-  <si>
-    <t>Verify all LEDs on GROVE modules are flashing</t>
+    <t>Program standard Arduino UNO bootloader onto ATMEGA328 using ISP header in preparation for shipping.</t>
   </si>
   <si>
     <t>FT_PROG</t>
@@ -3362,15 +3356,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:colOff>174240</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3902400</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:colOff>3994920</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>182520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3383,8 +3377,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="81000" y="16339320"/>
-          <a:ext cx="5085360" cy="5250240"/>
+          <a:off x="174240" y="16467480"/>
+          <a:ext cx="5084640" cy="5249520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3407,7 +3401,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="8:8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4810,7 +4804,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="1" sqref="8:8 B28"/>
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4937,10 +4931,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5336,7 +5330,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="21" t="s">
         <v>215</v>
       </c>
@@ -5344,43 +5338,43 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="22" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="21" t="s">
+    <row r="59" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="19" t="s">
         <v>219</v>
       </c>
       <c r="B59" s="22" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="B60" s="22" t="s">
+      <c r="B60" s="0" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="19" t="s">
+    <row r="61" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="21" t="s">
         <v>223</v>
       </c>
       <c r="B61" s="22" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="22" t="s">
         <v>226</v>
       </c>
     </row>
@@ -5400,15 +5394,15 @@
         <v>230</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="B65" s="22" t="s">
+      <c r="B65" s="0" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="21" t="s">
         <v>233</v>
       </c>
@@ -5417,25 +5411,18 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="21" t="s">
+      <c r="A67" s="21"/>
+      <c r="B67" s="0"/>
+    </row>
+    <row r="68" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B68" s="22" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="21"/>
-      <c r="B68" s="0"/>
-    </row>
-    <row r="69" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="B69" s="22" t="s">
-        <v>238</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A7:B7"/>

</xml_diff>